<commit_message>
xbee info and configuration profile for s2c router
</commit_message>
<xml_diff>
--- a/HIVE/relay/info/xbee_info.xlsx
+++ b/HIVE/relay/info/xbee_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all my files\downloads_current\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all my files\documents\uvm\5_masters\hive\github_directory\HIVE\relay\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CE2106-E46C-4D03-AF71-C5747F8EBC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC29805-C35B-4FFD-BB87-F46561678248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{811B69A6-7BAA-47F7-8449-D6A98DB96D93}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{811B69A6-7BAA-47F7-8449-D6A98DB96D93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={9CEBB753-356C-4B05-92F4-85D18BBE23D9}</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{9CEBB753-356C-4B05-92F4-85D18BBE23D9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Setup as 1 coord, 2 relay, 3 end</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -147,6 +165,54 @@
   </si>
   <si>
     <t>1F4</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>4104F320</t>
+  </si>
+  <si>
+    <t>94_coord</t>
+  </si>
+  <si>
+    <t>4104F322</t>
+  </si>
+  <si>
+    <t>95_end</t>
+  </si>
+  <si>
+    <t>S2C (threadAnt)</t>
+  </si>
+  <si>
+    <t>S2C (pcbAnt)</t>
+  </si>
+  <si>
+    <t>S1 (pcbAnt)</t>
+  </si>
+  <si>
+    <t>422DBDC4</t>
+  </si>
+  <si>
+    <t>88_router</t>
+  </si>
+  <si>
+    <t>422DC0C4</t>
+  </si>
+  <si>
+    <t>89_router</t>
+  </si>
+  <si>
+    <t>JV</t>
+  </si>
+  <si>
+    <t>96_router</t>
+  </si>
+  <si>
+    <t>97_router</t>
+  </si>
+  <si>
+    <t>99_router</t>
   </si>
 </sst>
 </file>
@@ -182,18 +248,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="23">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -204,6 +345,45 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Brandon Gamble" id="{63701861-AAD2-4F9A-AA46-A629DA70D705}" userId="S::bgamble@uvm.edu::72aa53af-923d-46b6-a293-3247b47d64c0" providerId="AD"/>
+</personList>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8266905B-4801-4118-B402-E0A40CDD2BC9}" name="Table1" displayName="Table1" ref="A2:U15" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A2:U15" xr:uid="{8266905B-4801-4118-B402-E0A40CDD2BC9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:U11">
+    <sortCondition ref="A2:A15"/>
+  </sortState>
+  <tableColumns count="21">
+    <tableColumn id="1" xr3:uid="{C23D5EF9-DF7F-4225-85F1-8152BF153E54}" name="ID" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{BA799C2E-3FE6-4567-B469-F3D4F073A6B9}" name="Model" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{A57567E2-8203-41A7-A70F-7EE86611F594}" name="CH" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{F5492253-D0DC-4491-8373-F6B255DD3522}" name="PAN ID" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{6901A33B-6D0E-4D3D-AF2E-4EECC1DB24D2}" name="SH" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{18B4FF2B-CD39-433F-B5B0-F47E06E3B602}" name="SL" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{01D1CCE1-5AE9-45D9-8888-4835DE4DFE77}" name="DH" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{CC97946A-8971-4E05-829D-2C6FC07FCBED}" name="DL" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{84290730-8393-4B28-A40F-5C764E3897FC}" name="MM" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{DCF09AF7-1383-467A-A491-F87D2D479375}" name="CE (coord enable)" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{E328F024-F86B-4859-896C-ADA2322B4F6B}" name="JV" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{B9CDBFEC-FA35-496F-9E03-D470F80ADE69}" name="NI" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{64039CB5-4224-4F8F-B856-C4192E70249B}" name="PL" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{193B10A1-FAFB-4FCB-BEDD-3098D3EFA902}" name="CA" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{1B28CD53-48F1-46BB-82E0-44354835CFB6}" name="SM" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{71B28181-F5C2-4D5D-8CBA-4FDBE988FFB6}" name="SP" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{6DCB4C35-A54F-4B6F-9229-1653BF1E96EA}" name="BD" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{4D9413CE-37FD-4FAC-87CE-88F7474BB903}" name="NB" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{732D288A-D450-4ECF-A388-347B6E7CE317}" name="RO" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{A2AFCFE4-E0AC-4E3E-B386-6C14EB052372}" name="AP" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{F958A014-46FF-42F8-969E-3641B45EEF17}" name="SO" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -521,349 +701,802 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A3" dT="2024-12-04T18:28:49.34" personId="{63701861-AAD2-4F9A-AA46-A629DA70D705}" id="{9CEBB753-356C-4B05-92F4-85D18BBE23D9}">
+    <text>Setup as 1 coord, 2 relay, 3 end</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C958D8FD-ED38-4072-847E-9B96E34E794A}">
-  <dimension ref="A1:S6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C958D8FD-ED38-4072-847E-9B96E34E794A}">
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="19.42578125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
-    <col min="11" max="12" width="9.140625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="1"/>
-    <col min="15" max="18" width="9.140625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="19.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="1"/>
+    <col min="13" max="14" width="9.140625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.140625" style="1"/>
+    <col min="17" max="20" width="9.140625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="3" t="s">
+    <row r="1" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="H1" s="2"/>
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>3332</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
         <v>4</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
       <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
         <v>38400</v>
       </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
         <v>3</v>
       </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>3332</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="1">
+      <c r="M4" s="1">
         <v>4</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
       <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
         <v>38400</v>
       </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
         <v>3</v>
       </c>
-      <c r="R4" s="1">
-        <v>0</v>
-      </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>3332</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="K5" s="1">
-        <v>4</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="M5" s="1">
         <v>4</v>
       </c>
       <c r="N5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="1">
+        <v>4</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O5" s="1">
+      <c r="Q5" s="1">
         <v>38400</v>
       </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
         <v>3</v>
       </c>
-      <c r="R5" s="1">
-        <v>0</v>
-      </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>3332</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="1">
+      <c r="M6" s="1">
         <v>4</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
       <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
         <v>38400</v>
       </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1">
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
         <v>3</v>
       </c>
-      <c r="R6" s="1">
-        <v>0</v>
-      </c>
-      <c r="S6" s="1">
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>88</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="1">
+        <v>4</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>38400</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>3</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>89</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="1">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="1">
+        <v>4</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>38400</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>3</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>93</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>94</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="1">
+        <v>4</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>38400</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>3</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>95</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" s="1">
+        <v>4</v>
+      </c>
+      <c r="O11" s="1">
+        <v>4</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>38400</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>3</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>96</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="1">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" s="1">
+        <v>4</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>38400</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>3</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>97</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" s="1">
+        <v>4</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>38400</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>3</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0</v>
+      </c>
+      <c r="U13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>98</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>99</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M15" s="1">
+        <v>4</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>38400</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1">
+        <v>3</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0</v>
+      </c>
+      <c r="U15" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="O1:R1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>